<commit_message>
updated, conversion to .db works
</commit_message>
<xml_diff>
--- a/rozklasowany/excelki/cases/combined/combined.xlsx
+++ b/rozklasowany/excelki/cases/combined/combined.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,11 +422,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="60" customWidth="1" min="1" max="1"/>
-    <col width="37" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="42" customWidth="1" min="4" max="4"/>
     <col width="30" customWidth="1" min="5" max="5"/>
-    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="17" customWidth="1" min="8" max="8"/>
   </cols>
@@ -439,304 +439,304 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>filename</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>surname</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>surname</t>
+          <t>university</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>university</t>
+          <t>bank account</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>bank account</t>
+          <t>currency</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>amount</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>amount</t>
+          <t>case number</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>combined.xlsx</t>
+          <t>Ella_Allen_University of Opole.xlsx</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ella_Allen_University of Opole.xlsx</t>
+          <t>Ella</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ella</t>
+          <t>Allen</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Allen</t>
+          <t>University of Opole</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>University of Opole</t>
+          <t>HU12345678901234567890123456</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>HU12345678901234567890123456</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>HUF</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="G2" t="n">
         <v>3456789.01</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>XLxFodWStBq9vqp</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ella_Allen_University of Opole.xlsx</t>
+          <t>Fiona_Garcia_AGH University of Science and Technology.xlsx</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ella</t>
+          <t>Fiona</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Allen</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>University of Opole</t>
+          <t>AGH University of Science and Technology</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>HU12345678901234567890123456</t>
+          <t>AU90123456789012345678901234</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>HUF</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>3456789.01</v>
+        <v>2109.87</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>XLxFodWStBq9vqp</t>
+          <t>TSSqJTgQscU3xRk</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Fiona_Garcia_AGH University of Science and Technology.xlsx</t>
+          <t>Jack_Adams_University of Innsbruck.xlsx</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fiona</t>
+          <t>Jack</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Adams</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>AGH University of Science and Technology</t>
+          <t>University of Innsbruck</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>AU90123456789012345678901234</t>
+          <t>CH56789012345678901234567890</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2109.87</v>
+        <v>8765.43</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>TSSqJTgQscU3xRk</t>
+          <t>20PHrLFFPkjoFh3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jack_Adams_University of Innsbruck.xlsx</t>
+          <t>Kevin_Hernandez_Silesian University of Technology.xlsx</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jack</t>
+          <t>Kevin</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Adams</t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>University of Innsbruck</t>
+          <t>Silesian University of Technology</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CH56789012345678901234567890</t>
+          <t>DK56789012345678901234567890</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>DKK</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>8765.43</v>
+        <v>54321.09</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>20PHrLFFPkjoFh3</t>
+          <t>IntCHCcO5hVBx7F</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kevin_Hernandez_Silesian University of Technology.xlsx</t>
+          <t>Olivia_Roberts_University of Bern.xlsx</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kevin</t>
+          <t>Olivia</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Roberts</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Silesian University of Technology</t>
+          <t>University of Bern</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>DK56789012345678901234567890</t>
+          <t>JP12345678901234567890</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DKK</t>
+          <t>JPY</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>54321.09</v>
+        <v>876543.21</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>IntCHCcO5hVBx7F</t>
+          <t>PsvOIOwtWHkuhak</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Olivia_Roberts_University of Bern.xlsx</t>
+          <t>Patricia_Thomas_University of Silesia.xlsx</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Olivia</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Roberts</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>University of Bern</t>
+          <t>University of Silesia</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>JP12345678901234567890</t>
+          <t>PT12345678901234567890123456</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>JPY</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>876543.21</v>
+        <v>7654.32</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>PsvOIOwtWHkuhak</t>
+          <t>azdzUIGGaiGBDMW</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Patricia_Thomas_University of Silesia.xlsx</t>
+          <t>Ursula_Lee_Opole University.xlsx</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Ursula</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>University of Silesia</t>
+          <t>Opole University</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>PT12345678901234567890123456</t>
+          <t>LU90123456789012345678901234</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -745,38 +745,38 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>7654.32</v>
+        <v>9876.540000000001</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>azdzUIGGaiGBDMW</t>
+          <t>RUk3wecSSbPhWC0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ursula_Lee_Opole University.xlsx</t>
+          <t>Zane_Clark_University of Economics in Katowice.xlsx</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ursula</t>
+          <t>Zane</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Clark</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Opole University</t>
+          <t>University of Economics in Katowice</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LU90123456789012345678901234</t>
+          <t>EE56789012345678901234567890</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -785,49 +785,9 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>9876.540000000001</v>
+        <v>6543.21</v>
       </c>
       <c r="H9" t="inlineStr">
-        <is>
-          <t>RUk3wecSSbPhWC0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Zane_Clark_University of Economics in Katowice.xlsx</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Zane</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Clark</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>University of Economics in Katowice</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>EE56789012345678901234567890</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>6543.21</v>
-      </c>
-      <c r="H10" t="inlineStr">
         <is>
           <t>Ki1E2GL7fuVqd1n</t>
         </is>

</xml_diff>